<commit_message>
Sprint grading file added, updated backlog
</commit_message>
<xml_diff>
--- a/JSON tools.xlsx
+++ b/JSON tools.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t xml:space="preserve">JSON tools</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t xml:space="preserve">Creating documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Classes documentation</t>
   </si>
   <si>
     <t xml:space="preserve">Transitioning from excel to GitHub projects</t>
@@ -261,45 +267,53 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -604,21 +618,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="95.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -646,140 +660,140 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="21.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="25.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="58.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="21.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="25.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="58.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -802,224 +816,246 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C41"/>
+  <dimension ref="A2:C43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="45.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="48.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="45.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="48.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="33"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="66.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="C8" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="6" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="C13" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4" t="s">
+      <c r="C15" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="C16" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4" t="s">
+      <c r="C18" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="C19" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4" t="s">
+      <c r="C21" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="68.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="C22" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="6" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="6" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="6" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
+      <c r="C31" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="5" t="n">
-        <v>1</v>
-      </c>
+      <c r="C32" s="6" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="12" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="5" t="n">
+      <c r="A35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C37" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="6" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
     <row r="41" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="5" t="n">
+      <c r="B41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>